<commit_message>
New report for Angola
</commit_message>
<xml_diff>
--- a/reports/Angola_exports_products_HS-AG6-2007-2022.xlsx
+++ b/reports/Angola_exports_products_HS-AG6-2007-2022.xlsx
@@ -256,19 +256,19 @@
     <t>HS</t>
   </si>
   <si>
-    <t>030219</t>
+    <t>090111</t>
   </si>
   <si>
-    <t>090111</t>
+    <t>710221</t>
+  </si>
+  <si>
+    <t>030219</t>
   </si>
   <si>
     <t>270740</t>
   </si>
   <si>
     <t>270900</t>
-  </si>
-  <si>
-    <t>710221</t>
   </si>
   <si>
     <t>440310</t>
@@ -298,22 +298,19 @@
     <t>890590</t>
   </si>
   <si>
-    <t>Fish; salmonidae, fresh or chilled, n.e.s. in item no. 0302.1 (excluding fillets, livers, roes and other fish meat of heading no. 0304)</t>
+    <t>Coffee; not roasted or decaffeinated</t>
   </si>
   <si>
-    <t>Coffee; not roasted or decaffeinated</t>
+    <t>Diamonds; industrial, unworked or simply sawn, cleaved or bruted, but not mounted or set</t>
+  </si>
+  <si>
+    <t>Fish; salmonidae, fresh or chilled, n.e.c. in item no. 0302.1 (excluding fillets, livers, roes and other fish meat of heading no. 0304)</t>
   </si>
   <si>
     <t>Oils and products of the distillation of high temperature coal tar; naphthalene</t>
   </si>
   <si>
     <t>Oils; petroleum oils and oils obtained from bituminous minerals, crude</t>
-  </si>
-  <si>
-    <t>Diamonds; industrial, unworked or simply sawn, cleaved or bruted, but not mounted or set</t>
-  </si>
-  <si>
-    <t>Fish; salmonidae, fresh or chilled, n.e.c. in item no. 0302.1 (excluding fillets, livers, roes and other fish meat of heading no. 0304)</t>
   </si>
   <si>
     <t>Wood; in the rough, whether or not stripped of bark or sapwood, or roughly squared; treated with paint, stains, creosote or other preservatives</t>
@@ -323,6 +320,9 @@
   </si>
   <si>
     <t>Marble and travertine; merely cut, by sawing or otherwise, into blocks or slabs of a rectangular (including square) shape, having a specific gravity of 2.5 or more</t>
+  </si>
+  <si>
+    <t>Fish; salmonidae, fresh or chilled, n.e.s. in item no. 0302.1 (excluding fillets, livers, roes and other fish meat of heading no. 0304)</t>
   </si>
   <si>
     <t>Floating or submersible drilling or production platforms</t>
@@ -996,7 +996,7 @@
         <v>115</v>
       </c>
       <c r="AF2">
-        <v>7000343</v>
+        <v>238878000</v>
       </c>
       <c r="AG2" t="b">
         <v>0</v>
@@ -1011,7 +1011,7 @@
         <v>0</v>
       </c>
       <c r="AL2">
-        <v>7000343</v>
+        <v>238878000</v>
       </c>
       <c r="AM2" t="b">
         <v>0</v>
@@ -1020,10 +1020,10 @@
         <v>0</v>
       </c>
       <c r="AQ2">
-        <v>42575360</v>
+        <v>413269</v>
       </c>
       <c r="AR2">
-        <v>42575360</v>
+        <v>413269</v>
       </c>
       <c r="AS2">
         <v>0</v>
@@ -1035,19 +1035,19 @@
         <v>0</v>
       </c>
       <c r="AV2">
-        <v>42575360</v>
+        <v>413269</v>
       </c>
       <c r="AW2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AX2">
-        <v>0.0009637278523364407</v>
+        <v>9.354679462657005E-06</v>
       </c>
       <c r="AY2">
         <v>44177783071</v>
       </c>
       <c r="AZ2">
-        <v>0.0009637278523364407</v>
+        <v>9.354679462657005E-06</v>
       </c>
     </row>
     <row r="3" spans="1:52">
@@ -1139,13 +1139,13 @@
         <v>114</v>
       </c>
       <c r="AD3">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="AE3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AF3">
-        <v>238878000</v>
+        <v>9077348</v>
       </c>
       <c r="AG3" t="b">
         <v>0</v>
@@ -1160,22 +1160,22 @@
         <v>0</v>
       </c>
       <c r="AL3">
-        <v>238878000</v>
+        <v>88667</v>
       </c>
       <c r="AM3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO3" t="b">
         <v>0</v>
       </c>
       <c r="AQ3">
-        <v>413269</v>
+        <v>1181943962</v>
       </c>
       <c r="AR3">
-        <v>413269</v>
+        <v>1181943962</v>
       </c>
       <c r="AS3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AT3" t="b">
         <v>1</v>
@@ -1184,19 +1184,19 @@
         <v>0</v>
       </c>
       <c r="AV3">
-        <v>413269</v>
+        <v>1181943962</v>
       </c>
       <c r="AW3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AX3">
-        <v>9.354679462657005E-06</v>
+        <v>0.02675426152780114</v>
       </c>
       <c r="AY3">
         <v>44177783071</v>
       </c>
       <c r="AZ3">
-        <v>9.354679462657005E-06</v>
+        <v>0.02675426152780114</v>
       </c>
     </row>
     <row r="4" spans="1:52">
@@ -1207,16 +1207,16 @@
         <v>53</v>
       </c>
       <c r="C4">
-        <v>20070101</v>
+        <v>20090101</v>
       </c>
       <c r="D4">
-        <v>2007</v>
+        <v>2009</v>
       </c>
       <c r="E4">
         <v>52</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G4">
         <v>24</v>
@@ -1252,7 +1252,7 @@
         <v>74</v>
       </c>
       <c r="R4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="S4" t="s">
         <v>79</v>
@@ -1294,7 +1294,7 @@
         <v>115</v>
       </c>
       <c r="AF4">
-        <v>1288118742</v>
+        <v>4899</v>
       </c>
       <c r="AG4" t="b">
         <v>0</v>
@@ -1309,7 +1309,7 @@
         <v>0</v>
       </c>
       <c r="AL4">
-        <v>1288118742</v>
+        <v>4899</v>
       </c>
       <c r="AM4" t="b">
         <v>0</v>
@@ -1318,10 +1318,10 @@
         <v>0</v>
       </c>
       <c r="AQ4">
-        <v>666333579</v>
+        <v>32169994</v>
       </c>
       <c r="AR4">
-        <v>666333579</v>
+        <v>32169994</v>
       </c>
       <c r="AS4">
         <v>0</v>
@@ -1333,19 +1333,19 @@
         <v>0</v>
       </c>
       <c r="AV4">
-        <v>666333579</v>
+        <v>32169994</v>
       </c>
       <c r="AW4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AX4">
-        <v>0.01508300174160181</v>
+        <v>0.0007915959564608788</v>
       </c>
       <c r="AY4">
-        <v>44177783071</v>
+        <v>40639411732</v>
       </c>
       <c r="AZ4">
-        <v>0.01508300174160181</v>
+        <v>0.0007915959564608788</v>
       </c>
     </row>
     <row r="5" spans="1:52">
@@ -1356,16 +1356,16 @@
         <v>53</v>
       </c>
       <c r="C5">
-        <v>20070101</v>
+        <v>20090101</v>
       </c>
       <c r="D5">
-        <v>2007</v>
+        <v>2009</v>
       </c>
       <c r="E5">
         <v>52</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G5">
         <v>24</v>
@@ -1401,7 +1401,7 @@
         <v>74</v>
       </c>
       <c r="R5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="S5" t="s">
         <v>79</v>
@@ -1410,10 +1410,10 @@
         <v>1</v>
       </c>
       <c r="U5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="V5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="W5">
         <v>6</v>
@@ -1443,7 +1443,7 @@
         <v>115</v>
       </c>
       <c r="AF5">
-        <v>96117049344</v>
+        <v>422425000</v>
       </c>
       <c r="AG5" t="b">
         <v>0</v>
@@ -1458,7 +1458,7 @@
         <v>0</v>
       </c>
       <c r="AL5">
-        <v>96117049344</v>
+        <v>422425000</v>
       </c>
       <c r="AM5" t="b">
         <v>0</v>
@@ -1467,10 +1467,10 @@
         <v>0</v>
       </c>
       <c r="AQ5">
-        <v>42286185648</v>
+        <v>810420</v>
       </c>
       <c r="AR5">
-        <v>42286185648</v>
+        <v>810420</v>
       </c>
       <c r="AS5">
         <v>0</v>
@@ -1482,19 +1482,19 @@
         <v>0</v>
       </c>
       <c r="AV5">
-        <v>42286185648</v>
+        <v>810420</v>
       </c>
       <c r="AW5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AX5">
-        <v>0.9571821560181069</v>
+        <v>1.99417256663158E-05</v>
       </c>
       <c r="AY5">
-        <v>44177783071</v>
+        <v>40639411732</v>
       </c>
       <c r="AZ5">
-        <v>0.9571821560181069</v>
+        <v>1.99417256663158E-05</v>
       </c>
     </row>
     <row r="6" spans="1:52">
@@ -1505,16 +1505,16 @@
         <v>53</v>
       </c>
       <c r="C6">
-        <v>20070101</v>
+        <v>20090101</v>
       </c>
       <c r="D6">
-        <v>2007</v>
+        <v>2009</v>
       </c>
       <c r="E6">
         <v>52</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G6">
         <v>24</v>
@@ -1550,7 +1550,7 @@
         <v>74</v>
       </c>
       <c r="R6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="S6" t="s">
         <v>79</v>
@@ -1559,10 +1559,10 @@
         <v>1</v>
       </c>
       <c r="U6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="V6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="W6">
         <v>6</v>
@@ -1592,7 +1592,7 @@
         <v>116</v>
       </c>
       <c r="AF6">
-        <v>9077348</v>
+        <v>9239269</v>
       </c>
       <c r="AG6" t="b">
         <v>0</v>
@@ -1607,7 +1607,7 @@
         <v>0</v>
       </c>
       <c r="AL6">
-        <v>88667</v>
+        <v>41375</v>
       </c>
       <c r="AM6" t="b">
         <v>1</v>
@@ -1616,10 +1616,10 @@
         <v>0</v>
       </c>
       <c r="AQ6">
-        <v>1181943962</v>
+        <v>813613812</v>
       </c>
       <c r="AR6">
-        <v>1181943962</v>
+        <v>813613812</v>
       </c>
       <c r="AS6">
         <v>4</v>
@@ -1631,19 +1631,19 @@
         <v>0</v>
       </c>
       <c r="AV6">
-        <v>1181943962</v>
+        <v>813613812</v>
       </c>
       <c r="AW6">
         <v>2</v>
       </c>
       <c r="AX6">
-        <v>0.02675426152780114</v>
+        <v>0.02002031469760055</v>
       </c>
       <c r="AY6">
-        <v>44177783071</v>
+        <v>40639411732</v>
       </c>
       <c r="AZ6">
-        <v>0.02675426152780114</v>
+        <v>0.02002031469760055</v>
       </c>
     </row>
     <row r="7" spans="1:52">
@@ -1654,16 +1654,16 @@
         <v>53</v>
       </c>
       <c r="C7">
-        <v>20090101</v>
+        <v>20100101</v>
       </c>
       <c r="D7">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="E7">
         <v>52</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G7">
         <v>24</v>
@@ -1708,10 +1708,10 @@
         <v>1</v>
       </c>
       <c r="U7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="V7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="W7">
         <v>6</v>
@@ -1741,7 +1741,7 @@
         <v>115</v>
       </c>
       <c r="AF7">
-        <v>4899</v>
+        <v>446705</v>
       </c>
       <c r="AG7" t="b">
         <v>0</v>
@@ -1756,7 +1756,7 @@
         <v>0</v>
       </c>
       <c r="AL7">
-        <v>4899</v>
+        <v>446705</v>
       </c>
       <c r="AM7" t="b">
         <v>0</v>
@@ -1765,10 +1765,10 @@
         <v>0</v>
       </c>
       <c r="AQ7">
-        <v>32169994</v>
+        <v>28075125</v>
       </c>
       <c r="AR7">
-        <v>32169994</v>
+        <v>28075125</v>
       </c>
       <c r="AS7">
         <v>0</v>
@@ -1780,19 +1780,19 @@
         <v>0</v>
       </c>
       <c r="AV7">
-        <v>32169994</v>
+        <v>28075125</v>
       </c>
       <c r="AW7">
         <v>4</v>
       </c>
       <c r="AX7">
-        <v>0.0007915959564608788</v>
+        <v>0.0005336247198489608</v>
       </c>
       <c r="AY7">
-        <v>40639411732</v>
+        <v>52612114761</v>
       </c>
       <c r="AZ7">
-        <v>0.0007915959564608788</v>
+        <v>0.0005336247198489608</v>
       </c>
     </row>
     <row r="8" spans="1:52">
@@ -1803,16 +1803,16 @@
         <v>53</v>
       </c>
       <c r="C8">
-        <v>20090101</v>
+        <v>20100101</v>
       </c>
       <c r="D8">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="E8">
         <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G8">
         <v>24</v>
@@ -1857,10 +1857,10 @@
         <v>1</v>
       </c>
       <c r="U8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="V8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W8">
         <v>6</v>
@@ -1890,7 +1890,7 @@
         <v>115</v>
       </c>
       <c r="AF8">
-        <v>422425000</v>
+        <v>304085008</v>
       </c>
       <c r="AG8" t="b">
         <v>0</v>
@@ -1905,7 +1905,7 @@
         <v>0</v>
       </c>
       <c r="AL8">
-        <v>422425000</v>
+        <v>304085008</v>
       </c>
       <c r="AM8" t="b">
         <v>0</v>
@@ -1914,10 +1914,10 @@
         <v>0</v>
       </c>
       <c r="AQ8">
-        <v>810420</v>
+        <v>569625</v>
       </c>
       <c r="AR8">
-        <v>810420</v>
+        <v>569625</v>
       </c>
       <c r="AS8">
         <v>0</v>
@@ -1929,19 +1929,19 @@
         <v>0</v>
       </c>
       <c r="AV8">
-        <v>810420</v>
+        <v>569625</v>
       </c>
       <c r="AW8">
         <v>5</v>
       </c>
       <c r="AX8">
-        <v>1.99417256663158E-05</v>
+        <v>1.082687899141907E-05</v>
       </c>
       <c r="AY8">
-        <v>40639411732</v>
+        <v>52612114761</v>
       </c>
       <c r="AZ8">
-        <v>1.99417256663158E-05</v>
+        <v>1.082687899141907E-05</v>
       </c>
     </row>
     <row r="9" spans="1:52">
@@ -1952,16 +1952,16 @@
         <v>53</v>
       </c>
       <c r="C9">
-        <v>20090101</v>
+        <v>20100101</v>
       </c>
       <c r="D9">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="E9">
         <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G9">
         <v>24</v>
@@ -2006,10 +2006,10 @@
         <v>1</v>
       </c>
       <c r="U9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="V9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W9">
         <v>6</v>
@@ -2033,13 +2033,13 @@
         <v>114</v>
       </c>
       <c r="AD9">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="AE9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AF9">
-        <v>1222619362</v>
+        <v>8425088</v>
       </c>
       <c r="AG9" t="b">
         <v>0</v>
@@ -2053,9 +2053,6 @@
       <c r="AK9" t="b">
         <v>0</v>
       </c>
-      <c r="AL9">
-        <v>1222619362</v>
-      </c>
       <c r="AM9" t="b">
         <v>0</v>
       </c>
@@ -2063,10 +2060,10 @@
         <v>0</v>
       </c>
       <c r="AQ9">
-        <v>530171435</v>
+        <v>1072039839</v>
       </c>
       <c r="AR9">
-        <v>530171435</v>
+        <v>1072039839</v>
       </c>
       <c r="AS9">
         <v>0</v>
@@ -2078,19 +2075,19 @@
         <v>0</v>
       </c>
       <c r="AV9">
-        <v>530171435</v>
+        <v>1072039839</v>
       </c>
       <c r="AW9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AX9">
-        <v>0.01304574580203719</v>
+        <v>0.02037629249213672</v>
       </c>
       <c r="AY9">
-        <v>40639411732</v>
+        <v>52612114761</v>
       </c>
       <c r="AZ9">
-        <v>0.01304574580203719</v>
+        <v>0.02037629249213672</v>
       </c>
     </row>
     <row r="10" spans="1:52">
@@ -2101,16 +2098,16 @@
         <v>53</v>
       </c>
       <c r="C10">
-        <v>20090101</v>
+        <v>20110101</v>
       </c>
       <c r="D10">
-        <v>2009</v>
+        <v>2011</v>
       </c>
       <c r="E10">
         <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G10">
         <v>24</v>
@@ -2155,10 +2152,10 @@
         <v>1</v>
       </c>
       <c r="U10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="W10">
         <v>6</v>
@@ -2188,7 +2185,7 @@
         <v>115</v>
       </c>
       <c r="AF10">
-        <v>104186865776</v>
+        <v>2748140</v>
       </c>
       <c r="AG10" t="b">
         <v>0</v>
@@ -2203,7 +2200,7 @@
         <v>0</v>
       </c>
       <c r="AL10">
-        <v>104186865776</v>
+        <v>2748140</v>
       </c>
       <c r="AM10" t="b">
         <v>0</v>
@@ -2212,10 +2209,10 @@
         <v>0</v>
       </c>
       <c r="AQ10">
-        <v>39262457163</v>
+        <v>24749315</v>
       </c>
       <c r="AR10">
-        <v>39262457163</v>
+        <v>24749315</v>
       </c>
       <c r="AS10">
         <v>0</v>
@@ -2227,19 +2224,19 @@
         <v>0</v>
       </c>
       <c r="AV10">
-        <v>39262457163</v>
+        <v>24749315</v>
       </c>
       <c r="AW10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AX10">
-        <v>0.9661177534241775</v>
+        <v>0.000372576958360596</v>
       </c>
       <c r="AY10">
-        <v>40639411732</v>
+        <v>66427390220</v>
       </c>
       <c r="AZ10">
-        <v>0.9661177534241775</v>
+        <v>0.000372576958360596</v>
       </c>
     </row>
     <row r="11" spans="1:52">
@@ -2250,16 +2247,16 @@
         <v>53</v>
       </c>
       <c r="C11">
-        <v>20090101</v>
+        <v>20110101</v>
       </c>
       <c r="D11">
-        <v>2009</v>
+        <v>2011</v>
       </c>
       <c r="E11">
         <v>52</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G11">
         <v>24</v>
@@ -2304,10 +2301,10 @@
         <v>1</v>
       </c>
       <c r="U11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="V11" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="W11">
         <v>6</v>
@@ -2331,13 +2328,13 @@
         <v>114</v>
       </c>
       <c r="AD11">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="AE11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AF11">
-        <v>9239269</v>
+        <v>444690008</v>
       </c>
       <c r="AG11" t="b">
         <v>0</v>
@@ -2352,22 +2349,22 @@
         <v>0</v>
       </c>
       <c r="AL11">
-        <v>41375</v>
+        <v>444690008</v>
       </c>
       <c r="AM11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO11" t="b">
         <v>0</v>
       </c>
       <c r="AQ11">
-        <v>813613812</v>
+        <v>960981</v>
       </c>
       <c r="AR11">
-        <v>813613812</v>
+        <v>960981</v>
       </c>
       <c r="AS11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AT11" t="b">
         <v>1</v>
@@ -2376,19 +2373,19 @@
         <v>0</v>
       </c>
       <c r="AV11">
-        <v>813613812</v>
+        <v>960981</v>
       </c>
       <c r="AW11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AX11">
-        <v>0.02002031469760055</v>
+        <v>1.446663788562729E-05</v>
       </c>
       <c r="AY11">
-        <v>40639411732</v>
+        <v>66427390220</v>
       </c>
       <c r="AZ11">
-        <v>0.02002031469760055</v>
+        <v>1.446663788562729E-05</v>
       </c>
     </row>
     <row r="12" spans="1:52">
@@ -2399,16 +2396,16 @@
         <v>53</v>
       </c>
       <c r="C12">
-        <v>20100101</v>
+        <v>20110101</v>
       </c>
       <c r="D12">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="E12">
         <v>52</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G12">
         <v>24</v>
@@ -2453,10 +2450,10 @@
         <v>1</v>
       </c>
       <c r="U12" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="V12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="W12">
         <v>6</v>
@@ -2486,7 +2483,7 @@
         <v>115</v>
       </c>
       <c r="AF12">
-        <v>446705</v>
+        <v>4640734059</v>
       </c>
       <c r="AG12" t="b">
         <v>0</v>
@@ -2501,7 +2498,7 @@
         <v>0</v>
       </c>
       <c r="AL12">
-        <v>446705</v>
+        <v>4640734059</v>
       </c>
       <c r="AM12" t="b">
         <v>0</v>
@@ -2510,10 +2507,10 @@
         <v>0</v>
       </c>
       <c r="AQ12">
-        <v>28075125</v>
+        <v>1052354330</v>
       </c>
       <c r="AR12">
-        <v>28075125</v>
+        <v>1052354330</v>
       </c>
       <c r="AS12">
         <v>0</v>
@@ -2525,19 +2522,19 @@
         <v>0</v>
       </c>
       <c r="AV12">
-        <v>28075125</v>
+        <v>1052354330</v>
       </c>
       <c r="AW12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AX12">
-        <v>0.0005336247198489608</v>
+        <v>0.01584217483954618</v>
       </c>
       <c r="AY12">
-        <v>52612114761</v>
+        <v>66427390220</v>
       </c>
       <c r="AZ12">
-        <v>0.0005336247198489608</v>
+        <v>0.01584217483954618</v>
       </c>
     </row>
     <row r="13" spans="1:52">
@@ -2548,16 +2545,16 @@
         <v>53</v>
       </c>
       <c r="C13">
-        <v>20100101</v>
+        <v>20110101</v>
       </c>
       <c r="D13">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="E13">
         <v>52</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G13">
         <v>24</v>
@@ -2602,10 +2599,10 @@
         <v>1</v>
       </c>
       <c r="U13" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="V13" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="W13">
         <v>6</v>
@@ -2635,7 +2632,7 @@
         <v>115</v>
       </c>
       <c r="AF13">
-        <v>304085008</v>
+        <v>92729565680</v>
       </c>
       <c r="AG13" t="b">
         <v>0</v>
@@ -2650,7 +2647,7 @@
         <v>0</v>
       </c>
       <c r="AL13">
-        <v>304085008</v>
+        <v>92729565680</v>
       </c>
       <c r="AM13" t="b">
         <v>0</v>
@@ -2659,10 +2656,10 @@
         <v>0</v>
       </c>
       <c r="AQ13">
-        <v>569625</v>
+        <v>64140141220</v>
       </c>
       <c r="AR13">
-        <v>569625</v>
+        <v>64140141220</v>
       </c>
       <c r="AS13">
         <v>0</v>
@@ -2674,19 +2671,19 @@
         <v>0</v>
       </c>
       <c r="AV13">
-        <v>569625</v>
+        <v>64140141220</v>
       </c>
       <c r="AW13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AX13">
-        <v>1.082687899141907E-05</v>
+        <v>0.9655676823607718</v>
       </c>
       <c r="AY13">
-        <v>52612114761</v>
+        <v>66427390220</v>
       </c>
       <c r="AZ13">
-        <v>1.082687899141907E-05</v>
+        <v>0.9655676823607718</v>
       </c>
     </row>
     <row r="14" spans="1:52">
@@ -2697,16 +2694,16 @@
         <v>53</v>
       </c>
       <c r="C14">
-        <v>20100101</v>
+        <v>20110101</v>
       </c>
       <c r="D14">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="E14">
         <v>52</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G14">
         <v>24</v>
@@ -2751,10 +2748,10 @@
         <v>1</v>
       </c>
       <c r="U14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="V14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W14">
         <v>6</v>
@@ -2778,13 +2775,13 @@
         <v>114</v>
       </c>
       <c r="AD14">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="AE14" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AF14">
-        <v>1876312685</v>
+        <v>8310143</v>
       </c>
       <c r="AG14" t="b">
         <v>0</v>
@@ -2799,22 +2796,22 @@
         <v>0</v>
       </c>
       <c r="AL14">
-        <v>1876312685</v>
+        <v>60986</v>
       </c>
       <c r="AM14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO14" t="b">
         <v>0</v>
       </c>
       <c r="AQ14">
-        <v>722363805</v>
+        <v>1209184374</v>
       </c>
       <c r="AR14">
-        <v>722363805</v>
+        <v>1209184374</v>
       </c>
       <c r="AS14">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AT14" t="b">
         <v>1</v>
@@ -2823,19 +2820,19 @@
         <v>0</v>
       </c>
       <c r="AV14">
-        <v>722363805</v>
+        <v>1209184374</v>
       </c>
       <c r="AW14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AX14">
-        <v>0.01372998991356777</v>
+        <v>0.01820309920343578</v>
       </c>
       <c r="AY14">
-        <v>52612114761</v>
+        <v>66427390220</v>
       </c>
       <c r="AZ14">
-        <v>0.01372998991356777</v>
+        <v>0.01820309920343578</v>
       </c>
     </row>
     <row r="15" spans="1:52">
@@ -2846,16 +2843,16 @@
         <v>53</v>
       </c>
       <c r="C15">
-        <v>20100101</v>
+        <v>20120101</v>
       </c>
       <c r="D15">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="E15">
         <v>52</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G15">
         <v>24</v>
@@ -2900,10 +2897,10 @@
         <v>1</v>
       </c>
       <c r="U15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="W15">
         <v>6</v>
@@ -2933,7 +2930,7 @@
         <v>115</v>
       </c>
       <c r="AF15">
-        <v>101134011072</v>
+        <v>8908</v>
       </c>
       <c r="AG15" t="b">
         <v>0</v>
@@ -2948,7 +2945,7 @@
         <v>0</v>
       </c>
       <c r="AL15">
-        <v>101134011072</v>
+        <v>8908</v>
       </c>
       <c r="AM15" t="b">
         <v>0</v>
@@ -2957,10 +2954,10 @@
         <v>0</v>
       </c>
       <c r="AQ15">
-        <v>50788866848</v>
+        <v>43681174</v>
       </c>
       <c r="AR15">
-        <v>50788866848</v>
+        <v>43681174</v>
       </c>
       <c r="AS15">
         <v>0</v>
@@ -2972,19 +2969,19 @@
         <v>0</v>
       </c>
       <c r="AV15">
-        <v>50788866848</v>
+        <v>43681174</v>
       </c>
       <c r="AW15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AX15">
-        <v>0.965345473732002</v>
+        <v>0.0006164165629138081</v>
       </c>
       <c r="AY15">
-        <v>52612114761</v>
+        <v>70863076413</v>
       </c>
       <c r="AZ15">
-        <v>0.965345473732002</v>
+        <v>0.0006164165629138081</v>
       </c>
     </row>
     <row r="16" spans="1:52">
@@ -2995,16 +2992,16 @@
         <v>53</v>
       </c>
       <c r="C16">
-        <v>20100101</v>
+        <v>20120101</v>
       </c>
       <c r="D16">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="E16">
         <v>52</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G16">
         <v>24</v>
@@ -3049,10 +3046,10 @@
         <v>1</v>
       </c>
       <c r="U16" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="V16" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="W16">
         <v>6</v>
@@ -3076,13 +3073,13 @@
         <v>114</v>
       </c>
       <c r="AD16">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="AE16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AF16">
-        <v>8425088</v>
+        <v>5693435208</v>
       </c>
       <c r="AG16" t="b">
         <v>0</v>
@@ -3096,6 +3093,9 @@
       <c r="AK16" t="b">
         <v>0</v>
       </c>
+      <c r="AL16">
+        <v>5693435208</v>
+      </c>
       <c r="AM16" t="b">
         <v>0</v>
       </c>
@@ -3103,10 +3103,10 @@
         <v>0</v>
       </c>
       <c r="AQ16">
-        <v>1072039839</v>
+        <v>1047546</v>
       </c>
       <c r="AR16">
-        <v>1072039839</v>
+        <v>1047546</v>
       </c>
       <c r="AS16">
         <v>0</v>
@@ -3118,19 +3118,19 @@
         <v>0</v>
       </c>
       <c r="AV16">
-        <v>1072039839</v>
+        <v>1047546</v>
       </c>
       <c r="AW16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AX16">
-        <v>0.02037629249213672</v>
+        <v>1.478267742561379E-05</v>
       </c>
       <c r="AY16">
-        <v>52612114761</v>
+        <v>70863076413</v>
       </c>
       <c r="AZ16">
-        <v>0.02037629249213672</v>
+        <v>1.478267742561379E-05</v>
       </c>
     </row>
     <row r="17" spans="1:52">
@@ -3141,16 +3141,16 @@
         <v>53</v>
       </c>
       <c r="C17">
-        <v>20110101</v>
+        <v>20120101</v>
       </c>
       <c r="D17">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="E17">
         <v>52</v>
       </c>
       <c r="F17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G17">
         <v>24</v>
@@ -3195,10 +3195,10 @@
         <v>1</v>
       </c>
       <c r="U17" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="V17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="W17">
         <v>6</v>
@@ -3228,7 +3228,7 @@
         <v>115</v>
       </c>
       <c r="AF17">
-        <v>2748140</v>
+        <v>1082433526</v>
       </c>
       <c r="AG17" t="b">
         <v>0</v>
@@ -3243,7 +3243,7 @@
         <v>0</v>
       </c>
       <c r="AL17">
-        <v>2748140</v>
+        <v>1082433526</v>
       </c>
       <c r="AM17" t="b">
         <v>0</v>
@@ -3252,10 +3252,10 @@
         <v>0</v>
       </c>
       <c r="AQ17">
-        <v>24749315</v>
+        <v>844858002</v>
       </c>
       <c r="AR17">
-        <v>24749315</v>
+        <v>844858002</v>
       </c>
       <c r="AS17">
         <v>0</v>
@@ -3267,19 +3267,19 @@
         <v>0</v>
       </c>
       <c r="AV17">
-        <v>24749315</v>
+        <v>844858002</v>
       </c>
       <c r="AW17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AX17">
-        <v>0.000372576958360596</v>
+        <v>0.01192240084350909</v>
       </c>
       <c r="AY17">
-        <v>66427390220</v>
+        <v>70863076413</v>
       </c>
       <c r="AZ17">
-        <v>0.000372576958360596</v>
+        <v>0.01192240084350909</v>
       </c>
     </row>
     <row r="18" spans="1:52">
@@ -3290,16 +3290,16 @@
         <v>53</v>
       </c>
       <c r="C18">
-        <v>20110101</v>
+        <v>20120101</v>
       </c>
       <c r="D18">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="E18">
         <v>52</v>
       </c>
       <c r="F18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G18">
         <v>24</v>
@@ -3344,10 +3344,10 @@
         <v>1</v>
       </c>
       <c r="U18" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="V18" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="W18">
         <v>6</v>
@@ -3377,7 +3377,7 @@
         <v>115</v>
       </c>
       <c r="AF18">
-        <v>444690008</v>
+        <v>98137524704</v>
       </c>
       <c r="AG18" t="b">
         <v>0</v>
@@ -3392,7 +3392,7 @@
         <v>0</v>
       </c>
       <c r="AL18">
-        <v>444690008</v>
+        <v>98137524704</v>
       </c>
       <c r="AM18" t="b">
         <v>0</v>
@@ -3401,10 +3401,10 @@
         <v>0</v>
       </c>
       <c r="AQ18">
-        <v>960981</v>
+        <v>68863266749</v>
       </c>
       <c r="AR18">
-        <v>960981</v>
+        <v>68863266749</v>
       </c>
       <c r="AS18">
         <v>0</v>
@@ -3416,19 +3416,19 @@
         <v>0</v>
       </c>
       <c r="AV18">
-        <v>960981</v>
+        <v>68863266749</v>
       </c>
       <c r="AW18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AX18">
-        <v>1.446663788562729E-05</v>
+        <v>0.9717792429396541</v>
       </c>
       <c r="AY18">
-        <v>66427390220</v>
+        <v>70863076413</v>
       </c>
       <c r="AZ18">
-        <v>1.446663788562729E-05</v>
+        <v>0.9717792429396541</v>
       </c>
     </row>
     <row r="19" spans="1:52">
@@ -3439,16 +3439,16 @@
         <v>53</v>
       </c>
       <c r="C19">
-        <v>20110101</v>
+        <v>20120101</v>
       </c>
       <c r="D19">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="E19">
         <v>52</v>
       </c>
       <c r="F19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G19">
         <v>24</v>
@@ -3493,10 +3493,10 @@
         <v>1</v>
       </c>
       <c r="U19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="V19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W19">
         <v>6</v>
@@ -3520,13 +3520,13 @@
         <v>114</v>
       </c>
       <c r="AD19">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="AE19" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AF19">
-        <v>4640734059</v>
+        <v>8330995</v>
       </c>
       <c r="AG19" t="b">
         <v>0</v>
@@ -3540,9 +3540,6 @@
       <c r="AK19" t="b">
         <v>0</v>
       </c>
-      <c r="AL19">
-        <v>4640734059</v>
-      </c>
       <c r="AM19" t="b">
         <v>0</v>
       </c>
@@ -3550,10 +3547,10 @@
         <v>0</v>
       </c>
       <c r="AQ19">
-        <v>1052354330</v>
+        <v>1110222942</v>
       </c>
       <c r="AR19">
-        <v>1052354330</v>
+        <v>1110222942</v>
       </c>
       <c r="AS19">
         <v>0</v>
@@ -3565,19 +3562,19 @@
         <v>0</v>
       </c>
       <c r="AV19">
-        <v>1052354330</v>
+        <v>1110222942</v>
       </c>
       <c r="AW19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AX19">
-        <v>0.01584217483954618</v>
+        <v>0.01566715697649738</v>
       </c>
       <c r="AY19">
-        <v>66427390220</v>
+        <v>70863076413</v>
       </c>
       <c r="AZ19">
-        <v>0.01584217483954618</v>
+        <v>0.01566715697649738</v>
       </c>
     </row>
     <row r="20" spans="1:52">
@@ -3588,16 +3585,16 @@
         <v>53</v>
       </c>
       <c r="C20">
-        <v>20110101</v>
+        <v>20130101</v>
       </c>
       <c r="D20">
-        <v>2011</v>
+        <v>2013</v>
       </c>
       <c r="E20">
         <v>52</v>
       </c>
       <c r="F20" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G20">
         <v>24</v>
@@ -3675,7 +3672,7 @@
         <v>115</v>
       </c>
       <c r="AF20">
-        <v>92729565680</v>
+        <v>1373433564</v>
       </c>
       <c r="AG20" t="b">
         <v>0</v>
@@ -3690,7 +3687,7 @@
         <v>0</v>
       </c>
       <c r="AL20">
-        <v>92729565680</v>
+        <v>1373433564</v>
       </c>
       <c r="AM20" t="b">
         <v>0</v>
@@ -3699,10 +3696,10 @@
         <v>0</v>
       </c>
       <c r="AQ20">
-        <v>64140141220</v>
+        <v>1041210067</v>
       </c>
       <c r="AR20">
-        <v>64140141220</v>
+        <v>1041210067</v>
       </c>
       <c r="AS20">
         <v>0</v>
@@ -3714,19 +3711,19 @@
         <v>0</v>
       </c>
       <c r="AV20">
-        <v>64140141220</v>
+        <v>1041210067</v>
       </c>
       <c r="AW20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AX20">
-        <v>0.9655676823607718</v>
+        <v>0.01537691945783894</v>
       </c>
       <c r="AY20">
-        <v>66427390220</v>
+        <v>67712526547</v>
       </c>
       <c r="AZ20">
-        <v>0.9655676823607718</v>
+        <v>0.01537691945783894</v>
       </c>
     </row>
     <row r="21" spans="1:52">
@@ -3737,16 +3734,16 @@
         <v>53</v>
       </c>
       <c r="C21">
-        <v>20110101</v>
+        <v>20130101</v>
       </c>
       <c r="D21">
-        <v>2011</v>
+        <v>2013</v>
       </c>
       <c r="E21">
         <v>52</v>
       </c>
       <c r="F21" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G21">
         <v>24</v>
@@ -3818,13 +3815,13 @@
         <v>114</v>
       </c>
       <c r="AD21">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="AE21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AF21">
-        <v>8310143</v>
+        <v>96731363120</v>
       </c>
       <c r="AG21" t="b">
         <v>0</v>
@@ -3839,22 +3836,22 @@
         <v>0</v>
       </c>
       <c r="AL21">
-        <v>60986</v>
+        <v>96731363120</v>
       </c>
       <c r="AM21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO21" t="b">
         <v>0</v>
       </c>
       <c r="AQ21">
-        <v>1209184374</v>
+        <v>65464178236</v>
       </c>
       <c r="AR21">
-        <v>1209184374</v>
+        <v>65464178236</v>
       </c>
       <c r="AS21">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AT21" t="b">
         <v>1</v>
@@ -3863,19 +3860,19 @@
         <v>0</v>
       </c>
       <c r="AV21">
-        <v>1209184374</v>
+        <v>65464178236</v>
       </c>
       <c r="AW21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AX21">
-        <v>0.01820309920343578</v>
+        <v>0.966795681306628</v>
       </c>
       <c r="AY21">
-        <v>66427390220</v>
+        <v>67712526547</v>
       </c>
       <c r="AZ21">
-        <v>0.01820309920343578</v>
+        <v>0.966795681306628</v>
       </c>
     </row>
     <row r="22" spans="1:52">
@@ -3886,16 +3883,16 @@
         <v>53</v>
       </c>
       <c r="C22">
-        <v>20120101</v>
+        <v>20130101</v>
       </c>
       <c r="D22">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="E22">
         <v>52</v>
       </c>
       <c r="F22" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G22">
         <v>24</v>
@@ -3940,7 +3937,7 @@
         <v>1</v>
       </c>
       <c r="U22" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="V22" t="s">
         <v>99</v>
@@ -3967,13 +3964,13 @@
         <v>114</v>
       </c>
       <c r="AD22">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="AE22" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AF22">
-        <v>8908</v>
+        <v>4796</v>
       </c>
       <c r="AG22" t="b">
         <v>0</v>
@@ -3988,22 +3985,22 @@
         <v>0</v>
       </c>
       <c r="AL22">
-        <v>8908</v>
+        <v>2745138</v>
       </c>
       <c r="AM22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO22" t="b">
         <v>0</v>
       </c>
       <c r="AQ22">
-        <v>43681174</v>
+        <v>1336889</v>
       </c>
       <c r="AR22">
-        <v>43681174</v>
+        <v>1336889</v>
       </c>
       <c r="AS22">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AT22" t="b">
         <v>1</v>
@@ -4012,19 +4009,19 @@
         <v>0</v>
       </c>
       <c r="AV22">
-        <v>43681174</v>
+        <v>1336889</v>
       </c>
       <c r="AW22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AX22">
-        <v>0.0006164165629138081</v>
+        <v>1.974359942206633E-05</v>
       </c>
       <c r="AY22">
-        <v>70863076413</v>
+        <v>67712526547</v>
       </c>
       <c r="AZ22">
-        <v>0.0006164165629138081</v>
+        <v>1.974359942206633E-05</v>
       </c>
     </row>
     <row r="23" spans="1:52">
@@ -4035,16 +4032,16 @@
         <v>53</v>
       </c>
       <c r="C23">
-        <v>20120101</v>
+        <v>20130101</v>
       </c>
       <c r="D23">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="E23">
         <v>52</v>
       </c>
       <c r="F23" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G23">
         <v>24</v>
@@ -4089,10 +4086,10 @@
         <v>1</v>
       </c>
       <c r="U23" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="V23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="W23">
         <v>6</v>
@@ -4122,7 +4119,7 @@
         <v>115</v>
       </c>
       <c r="AF23">
-        <v>5693435208</v>
+        <v>2411343</v>
       </c>
       <c r="AG23" t="b">
         <v>0</v>
@@ -4137,7 +4134,7 @@
         <v>0</v>
       </c>
       <c r="AL23">
-        <v>5693435208</v>
+        <v>2411343</v>
       </c>
       <c r="AM23" t="b">
         <v>0</v>
@@ -4146,10 +4143,10 @@
         <v>0</v>
       </c>
       <c r="AQ23">
-        <v>1047546</v>
+        <v>49146741</v>
       </c>
       <c r="AR23">
-        <v>1047546</v>
+        <v>49146741</v>
       </c>
       <c r="AS23">
         <v>0</v>
@@ -4161,19 +4158,19 @@
         <v>0</v>
       </c>
       <c r="AV23">
-        <v>1047546</v>
+        <v>49146741</v>
       </c>
       <c r="AW23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AX23">
-        <v>1.478267742561379E-05</v>
+        <v>0.0007258146092936986</v>
       </c>
       <c r="AY23">
-        <v>70863076413</v>
+        <v>67712526547</v>
       </c>
       <c r="AZ23">
-        <v>1.478267742561379E-05</v>
+        <v>0.0007258146092936986</v>
       </c>
     </row>
     <row r="24" spans="1:52">
@@ -4184,16 +4181,16 @@
         <v>53</v>
       </c>
       <c r="C24">
-        <v>20120101</v>
+        <v>20130101</v>
       </c>
       <c r="D24">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="E24">
         <v>52</v>
       </c>
       <c r="F24" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G24">
         <v>24</v>
@@ -4238,10 +4235,10 @@
         <v>1</v>
       </c>
       <c r="U24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="V24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W24">
         <v>6</v>
@@ -4265,13 +4262,13 @@
         <v>114</v>
       </c>
       <c r="AD24">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="AE24" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AF24">
-        <v>1082433526</v>
+        <v>8577975</v>
       </c>
       <c r="AG24" t="b">
         <v>0</v>
@@ -4286,22 +4283,22 @@
         <v>0</v>
       </c>
       <c r="AL24">
-        <v>1082433526</v>
+        <v>39667</v>
       </c>
       <c r="AM24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO24" t="b">
         <v>0</v>
       </c>
       <c r="AQ24">
-        <v>844858002</v>
+        <v>1156063734</v>
       </c>
       <c r="AR24">
-        <v>844858002</v>
+        <v>1156063734</v>
       </c>
       <c r="AS24">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AT24" t="b">
         <v>1</v>
@@ -4310,19 +4307,19 @@
         <v>0</v>
       </c>
       <c r="AV24">
-        <v>844858002</v>
+        <v>1156063734</v>
       </c>
       <c r="AW24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AX24">
-        <v>0.01192240084350909</v>
+        <v>0.01707311472416501</v>
       </c>
       <c r="AY24">
-        <v>70863076413</v>
+        <v>67712526547</v>
       </c>
       <c r="AZ24">
-        <v>0.01192240084350909</v>
+        <v>0.01707311472416501</v>
       </c>
     </row>
     <row r="25" spans="1:52">
@@ -4333,16 +4330,16 @@
         <v>53</v>
       </c>
       <c r="C25">
-        <v>20120101</v>
+        <v>20140101</v>
       </c>
       <c r="D25">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="E25">
         <v>52</v>
       </c>
       <c r="F25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G25">
         <v>24</v>
@@ -4378,7 +4375,7 @@
         <v>74</v>
       </c>
       <c r="R25" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="S25" t="s">
         <v>79</v>
@@ -4387,10 +4384,10 @@
         <v>1</v>
       </c>
       <c r="U25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V25" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="W25">
         <v>6</v>
@@ -4420,7 +4417,7 @@
         <v>115</v>
       </c>
       <c r="AF25">
-        <v>98137524704</v>
+        <v>1469118</v>
       </c>
       <c r="AG25" t="b">
         <v>0</v>
@@ -4435,7 +4432,7 @@
         <v>0</v>
       </c>
       <c r="AL25">
-        <v>98137524704</v>
+        <v>1469118</v>
       </c>
       <c r="AM25" t="b">
         <v>0</v>
@@ -4444,10 +4441,10 @@
         <v>0</v>
       </c>
       <c r="AQ25">
-        <v>68863266749</v>
+        <v>48757176</v>
       </c>
       <c r="AR25">
-        <v>68863266749</v>
+        <v>48757176</v>
       </c>
       <c r="AS25">
         <v>0</v>
@@ -4459,19 +4456,19 @@
         <v>0</v>
       </c>
       <c r="AV25">
-        <v>68863266749</v>
+        <v>48757176</v>
       </c>
       <c r="AW25">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AX25">
-        <v>0.9717792429396541</v>
+        <v>0.0008310074515872638</v>
       </c>
       <c r="AY25">
-        <v>70863076413</v>
+        <v>58672369191</v>
       </c>
       <c r="AZ25">
-        <v>0.9717792429396541</v>
+        <v>0.0008310074515872638</v>
       </c>
     </row>
     <row r="26" spans="1:52">
@@ -4482,16 +4479,16 @@
         <v>53</v>
       </c>
       <c r="C26">
-        <v>20120101</v>
+        <v>20140101</v>
       </c>
       <c r="D26">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="E26">
         <v>52</v>
       </c>
       <c r="F26" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G26">
         <v>24</v>
@@ -4527,7 +4524,7 @@
         <v>74</v>
       </c>
       <c r="R26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="S26" t="s">
         <v>79</v>
@@ -4536,10 +4533,10 @@
         <v>1</v>
       </c>
       <c r="U26" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="V26" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="W26">
         <v>6</v>
@@ -4563,16 +4560,16 @@
         <v>114</v>
       </c>
       <c r="AD26">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="AE26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AF26">
-        <v>8330995</v>
+        <v>23201990</v>
       </c>
       <c r="AG26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH26">
         <v>-1</v>
@@ -4583,20 +4580,23 @@
       <c r="AK26" t="b">
         <v>0</v>
       </c>
+      <c r="AL26">
+        <v>23201990</v>
+      </c>
       <c r="AM26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO26" t="b">
         <v>0</v>
       </c>
       <c r="AQ26">
-        <v>1110222942</v>
+        <v>7199794</v>
       </c>
       <c r="AR26">
-        <v>1110222942</v>
+        <v>7199794</v>
       </c>
       <c r="AS26">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AT26" t="b">
         <v>1</v>
@@ -4605,19 +4605,19 @@
         <v>0</v>
       </c>
       <c r="AV26">
-        <v>1110222942</v>
+        <v>7199794</v>
       </c>
       <c r="AW26">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AX26">
-        <v>0.01566715697649738</v>
+        <v>0.0001227118335133535</v>
       </c>
       <c r="AY26">
-        <v>70863076413</v>
+        <v>58672369191</v>
       </c>
       <c r="AZ26">
-        <v>0.01566715697649738</v>
+        <v>0.0001227118335133535</v>
       </c>
     </row>
     <row r="27" spans="1:52">
@@ -4628,16 +4628,16 @@
         <v>53</v>
       </c>
       <c r="C27">
-        <v>20130101</v>
+        <v>20140101</v>
       </c>
       <c r="D27">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="E27">
         <v>52</v>
       </c>
       <c r="F27" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G27">
         <v>24</v>
@@ -4673,7 +4673,7 @@
         <v>74</v>
       </c>
       <c r="R27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="S27" t="s">
         <v>79</v>
@@ -4682,10 +4682,10 @@
         <v>1</v>
       </c>
       <c r="U27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="V27" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="W27">
         <v>6</v>
@@ -4715,7 +4715,7 @@
         <v>115</v>
       </c>
       <c r="AF27">
-        <v>1373433564</v>
+        <v>1351390566</v>
       </c>
       <c r="AG27" t="b">
         <v>0</v>
@@ -4730,7 +4730,7 @@
         <v>0</v>
       </c>
       <c r="AL27">
-        <v>1373433564</v>
+        <v>1351390566</v>
       </c>
       <c r="AM27" t="b">
         <v>0</v>
@@ -4739,10 +4739,10 @@
         <v>0</v>
       </c>
       <c r="AQ27">
-        <v>1041210067</v>
+        <v>896700136</v>
       </c>
       <c r="AR27">
-        <v>1041210067</v>
+        <v>896700136</v>
       </c>
       <c r="AS27">
         <v>0</v>
@@ -4754,19 +4754,19 @@
         <v>0</v>
       </c>
       <c r="AV27">
-        <v>1041210067</v>
+        <v>896700136</v>
       </c>
       <c r="AW27">
         <v>3</v>
       </c>
       <c r="AX27">
-        <v>0.01537691945783894</v>
+        <v>0.01528317585200818</v>
       </c>
       <c r="AY27">
-        <v>67712526547</v>
+        <v>58672369191</v>
       </c>
       <c r="AZ27">
-        <v>0.01537691945783894</v>
+        <v>0.01528317585200818</v>
       </c>
     </row>
     <row r="28" spans="1:52">
@@ -4777,16 +4777,16 @@
         <v>53</v>
       </c>
       <c r="C28">
-        <v>20130101</v>
+        <v>20140101</v>
       </c>
       <c r="D28">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="E28">
         <v>52</v>
       </c>
       <c r="F28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G28">
         <v>24</v>
@@ -4822,7 +4822,7 @@
         <v>74</v>
       </c>
       <c r="R28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="S28" t="s">
         <v>79</v>
@@ -4831,10 +4831,10 @@
         <v>1</v>
       </c>
       <c r="U28" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="V28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="W28">
         <v>6</v>
@@ -4864,7 +4864,7 @@
         <v>115</v>
       </c>
       <c r="AF28">
-        <v>96731363120</v>
+        <v>93460291176</v>
       </c>
       <c r="AG28" t="b">
         <v>0</v>
@@ -4879,7 +4879,7 @@
         <v>0</v>
       </c>
       <c r="AL28">
-        <v>96731363120</v>
+        <v>93460291176</v>
       </c>
       <c r="AM28" t="b">
         <v>0</v>
@@ -4888,10 +4888,10 @@
         <v>0</v>
       </c>
       <c r="AQ28">
-        <v>65464178236</v>
+        <v>56439535479</v>
       </c>
       <c r="AR28">
-        <v>65464178236</v>
+        <v>56439535479</v>
       </c>
       <c r="AS28">
         <v>0</v>
@@ -4903,19 +4903,19 @@
         <v>0</v>
       </c>
       <c r="AV28">
-        <v>65464178236</v>
+        <v>56439535479</v>
       </c>
       <c r="AW28">
         <v>1</v>
       </c>
       <c r="AX28">
-        <v>0.966795681306628</v>
+        <v>0.9619440335751347</v>
       </c>
       <c r="AY28">
-        <v>67712526547</v>
+        <v>58672369191</v>
       </c>
       <c r="AZ28">
-        <v>0.966795681306628</v>
+        <v>0.9619440335751347</v>
       </c>
     </row>
     <row r="29" spans="1:52">
@@ -4926,16 +4926,16 @@
         <v>53</v>
       </c>
       <c r="C29">
-        <v>20130101</v>
+        <v>20140101</v>
       </c>
       <c r="D29">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="E29">
         <v>52</v>
       </c>
       <c r="F29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G29">
         <v>24</v>
@@ -4971,7 +4971,7 @@
         <v>74</v>
       </c>
       <c r="R29" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="S29" t="s">
         <v>79</v>
@@ -4980,10 +4980,10 @@
         <v>1</v>
       </c>
       <c r="U29" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="V29" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="W29">
         <v>6</v>
@@ -5007,13 +5007,10 @@
         <v>114</v>
       </c>
       <c r="AD29">
-        <v>12</v>
+        <v>-1</v>
       </c>
       <c r="AE29" t="s">
-        <v>117</v>
-      </c>
-      <c r="AF29">
-        <v>4796</v>
+        <v>118</v>
       </c>
       <c r="AG29" t="b">
         <v>0</v>
@@ -5027,23 +5024,20 @@
       <c r="AK29" t="b">
         <v>0</v>
       </c>
-      <c r="AL29">
-        <v>2745138</v>
-      </c>
       <c r="AM29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO29" t="b">
         <v>0</v>
       </c>
       <c r="AQ29">
-        <v>1336889</v>
+        <v>1274009584</v>
       </c>
       <c r="AR29">
-        <v>1336889</v>
+        <v>1274009584</v>
       </c>
       <c r="AS29">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AT29" t="b">
         <v>1</v>
@@ -5052,19 +5046,19 @@
         <v>0</v>
       </c>
       <c r="AV29">
-        <v>1336889</v>
+        <v>1274009584</v>
       </c>
       <c r="AW29">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AX29">
-        <v>1.974359942206633E-05</v>
+        <v>0.02171396181143859</v>
       </c>
       <c r="AY29">
-        <v>67712526547</v>
+        <v>58672369191</v>
       </c>
       <c r="AZ29">
-        <v>1.974359942206633E-05</v>
+        <v>0.02171396181143859</v>
       </c>
     </row>
     <row r="30" spans="1:52">
@@ -5075,16 +5069,16 @@
         <v>53</v>
       </c>
       <c r="C30">
-        <v>20130101</v>
+        <v>20100101</v>
       </c>
       <c r="D30">
-        <v>2013</v>
+        <v>2010</v>
       </c>
       <c r="E30">
         <v>52</v>
       </c>
       <c r="F30" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G30">
         <v>24</v>
@@ -5129,10 +5123,10 @@
         <v>1</v>
       </c>
       <c r="U30" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="V30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="W30">
         <v>6</v>
@@ -5162,7 +5156,7 @@
         <v>115</v>
       </c>
       <c r="AF30">
-        <v>2411343</v>
+        <v>101134011072</v>
       </c>
       <c r="AG30" t="b">
         <v>0</v>
@@ -5177,7 +5171,7 @@
         <v>0</v>
       </c>
       <c r="AL30">
-        <v>2411343</v>
+        <v>101134011072</v>
       </c>
       <c r="AM30" t="b">
         <v>0</v>
@@ -5186,10 +5180,10 @@
         <v>0</v>
       </c>
       <c r="AQ30">
-        <v>49146741</v>
+        <v>50788866848</v>
       </c>
       <c r="AR30">
-        <v>49146741</v>
+        <v>50788866848</v>
       </c>
       <c r="AS30">
         <v>0</v>
@@ -5201,19 +5195,19 @@
         <v>0</v>
       </c>
       <c r="AV30">
-        <v>49146741</v>
+        <v>50788866848</v>
       </c>
       <c r="AW30">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AX30">
-        <v>0.0007258146092936986</v>
+        <v>0.965345473732002</v>
       </c>
       <c r="AY30">
-        <v>67712526547</v>
+        <v>52612114761</v>
       </c>
       <c r="AZ30">
-        <v>0.0007258146092936986</v>
+        <v>0.965345473732002</v>
       </c>
     </row>
     <row r="31" spans="1:52">
@@ -5224,16 +5218,16 @@
         <v>53</v>
       </c>
       <c r="C31">
-        <v>20130101</v>
+        <v>20100101</v>
       </c>
       <c r="D31">
-        <v>2013</v>
+        <v>2010</v>
       </c>
       <c r="E31">
         <v>52</v>
       </c>
       <c r="F31" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G31">
         <v>24</v>
@@ -5278,10 +5272,10 @@
         <v>1</v>
       </c>
       <c r="U31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="V31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="W31">
         <v>6</v>
@@ -5305,13 +5299,13 @@
         <v>114</v>
       </c>
       <c r="AD31">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="AE31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AF31">
-        <v>8577975</v>
+        <v>1876312685</v>
       </c>
       <c r="AG31" t="b">
         <v>0</v>
@@ -5326,22 +5320,22 @@
         <v>0</v>
       </c>
       <c r="AL31">
-        <v>39667</v>
+        <v>1876312685</v>
       </c>
       <c r="AM31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO31" t="b">
         <v>0</v>
       </c>
       <c r="AQ31">
-        <v>1156063734</v>
+        <v>722363805</v>
       </c>
       <c r="AR31">
-        <v>1156063734</v>
+        <v>722363805</v>
       </c>
       <c r="AS31">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AT31" t="b">
         <v>1</v>
@@ -5350,19 +5344,19 @@
         <v>0</v>
       </c>
       <c r="AV31">
-        <v>1156063734</v>
+        <v>722363805</v>
       </c>
       <c r="AW31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AX31">
-        <v>0.01707311472416501</v>
+        <v>0.01372998991356777</v>
       </c>
       <c r="AY31">
-        <v>67712526547</v>
+        <v>52612114761</v>
       </c>
       <c r="AZ31">
-        <v>0.01707311472416501</v>
+        <v>0.01372998991356777</v>
       </c>
     </row>
     <row r="32" spans="1:52">
@@ -5373,16 +5367,16 @@
         <v>53</v>
       </c>
       <c r="C32">
-        <v>20140101</v>
+        <v>20090101</v>
       </c>
       <c r="D32">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="E32">
         <v>52</v>
       </c>
       <c r="F32" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G32">
         <v>24</v>
@@ -5418,7 +5412,7 @@
         <v>74</v>
       </c>
       <c r="R32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S32" t="s">
         <v>79</v>
@@ -5427,10 +5421,10 @@
         <v>1</v>
       </c>
       <c r="U32" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="V32" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="W32">
         <v>6</v>
@@ -5460,7 +5454,7 @@
         <v>115</v>
       </c>
       <c r="AF32">
-        <v>1469118</v>
+        <v>104186865776</v>
       </c>
       <c r="AG32" t="b">
         <v>0</v>
@@ -5475,7 +5469,7 @@
         <v>0</v>
       </c>
       <c r="AL32">
-        <v>1469118</v>
+        <v>104186865776</v>
       </c>
       <c r="AM32" t="b">
         <v>0</v>
@@ -5484,10 +5478,10 @@
         <v>0</v>
       </c>
       <c r="AQ32">
-        <v>48757176</v>
+        <v>39262457163</v>
       </c>
       <c r="AR32">
-        <v>48757176</v>
+        <v>39262457163</v>
       </c>
       <c r="AS32">
         <v>0</v>
@@ -5499,19 +5493,19 @@
         <v>0</v>
       </c>
       <c r="AV32">
-        <v>48757176</v>
+        <v>39262457163</v>
       </c>
       <c r="AW32">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AX32">
-        <v>0.0008310074515872638</v>
+        <v>0.9661177534241775</v>
       </c>
       <c r="AY32">
-        <v>58672369191</v>
+        <v>40639411732</v>
       </c>
       <c r="AZ32">
-        <v>0.0008310074515872638</v>
+        <v>0.9661177534241775</v>
       </c>
     </row>
     <row r="33" spans="1:52">
@@ -5522,16 +5516,16 @@
         <v>53</v>
       </c>
       <c r="C33">
-        <v>20140101</v>
+        <v>20090101</v>
       </c>
       <c r="D33">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="E33">
         <v>52</v>
       </c>
       <c r="F33" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G33">
         <v>24</v>
@@ -5567,7 +5561,7 @@
         <v>74</v>
       </c>
       <c r="R33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S33" t="s">
         <v>79</v>
@@ -5576,10 +5570,10 @@
         <v>1</v>
       </c>
       <c r="U33" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="V33" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="W33">
         <v>6</v>
@@ -5609,10 +5603,10 @@
         <v>115</v>
       </c>
       <c r="AF33">
-        <v>23201990</v>
+        <v>1222619362</v>
       </c>
       <c r="AG33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH33">
         <v>-1</v>
@@ -5624,22 +5618,22 @@
         <v>0</v>
       </c>
       <c r="AL33">
-        <v>23201990</v>
+        <v>1222619362</v>
       </c>
       <c r="AM33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO33" t="b">
         <v>0</v>
       </c>
       <c r="AQ33">
-        <v>7199794</v>
+        <v>530171435</v>
       </c>
       <c r="AR33">
-        <v>7199794</v>
+        <v>530171435</v>
       </c>
       <c r="AS33">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AT33" t="b">
         <v>1</v>
@@ -5648,19 +5642,19 @@
         <v>0</v>
       </c>
       <c r="AV33">
-        <v>7199794</v>
+        <v>530171435</v>
       </c>
       <c r="AW33">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AX33">
-        <v>0.0001227118335133535</v>
+        <v>0.01304574580203719</v>
       </c>
       <c r="AY33">
-        <v>58672369191</v>
+        <v>40639411732</v>
       </c>
       <c r="AZ33">
-        <v>0.0001227118335133535</v>
+        <v>0.01304574580203719</v>
       </c>
     </row>
     <row r="34" spans="1:52">
@@ -5671,16 +5665,16 @@
         <v>53</v>
       </c>
       <c r="C34">
-        <v>20140101</v>
+        <v>20070101</v>
       </c>
       <c r="D34">
-        <v>2014</v>
+        <v>2007</v>
       </c>
       <c r="E34">
         <v>52</v>
       </c>
       <c r="F34" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G34">
         <v>24</v>
@@ -5716,7 +5710,7 @@
         <v>74</v>
       </c>
       <c r="R34" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S34" t="s">
         <v>79</v>
@@ -5725,10 +5719,10 @@
         <v>1</v>
       </c>
       <c r="U34" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="V34" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="W34">
         <v>6</v>
@@ -5758,7 +5752,7 @@
         <v>115</v>
       </c>
       <c r="AF34">
-        <v>1351390566</v>
+        <v>96117049344</v>
       </c>
       <c r="AG34" t="b">
         <v>0</v>
@@ -5773,7 +5767,7 @@
         <v>0</v>
       </c>
       <c r="AL34">
-        <v>1351390566</v>
+        <v>96117049344</v>
       </c>
       <c r="AM34" t="b">
         <v>0</v>
@@ -5782,10 +5776,10 @@
         <v>0</v>
       </c>
       <c r="AQ34">
-        <v>896700136</v>
+        <v>42286185648</v>
       </c>
       <c r="AR34">
-        <v>896700136</v>
+        <v>42286185648</v>
       </c>
       <c r="AS34">
         <v>0</v>
@@ -5797,19 +5791,19 @@
         <v>0</v>
       </c>
       <c r="AV34">
-        <v>896700136</v>
+        <v>42286185648</v>
       </c>
       <c r="AW34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AX34">
-        <v>0.01528317585200818</v>
+        <v>0.9571821560181069</v>
       </c>
       <c r="AY34">
-        <v>58672369191</v>
+        <v>44177783071</v>
       </c>
       <c r="AZ34">
-        <v>0.01528317585200818</v>
+        <v>0.9571821560181069</v>
       </c>
     </row>
     <row r="35" spans="1:52">
@@ -5820,16 +5814,16 @@
         <v>53</v>
       </c>
       <c r="C35">
-        <v>20140101</v>
+        <v>20070101</v>
       </c>
       <c r="D35">
-        <v>2014</v>
+        <v>2007</v>
       </c>
       <c r="E35">
         <v>52</v>
       </c>
       <c r="F35" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G35">
         <v>24</v>
@@ -5865,7 +5859,7 @@
         <v>74</v>
       </c>
       <c r="R35" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S35" t="s">
         <v>79</v>
@@ -5907,7 +5901,7 @@
         <v>115</v>
       </c>
       <c r="AF35">
-        <v>93460291176</v>
+        <v>1288118742</v>
       </c>
       <c r="AG35" t="b">
         <v>0</v>
@@ -5922,7 +5916,7 @@
         <v>0</v>
       </c>
       <c r="AL35">
-        <v>93460291176</v>
+        <v>1288118742</v>
       </c>
       <c r="AM35" t="b">
         <v>0</v>
@@ -5931,10 +5925,10 @@
         <v>0</v>
       </c>
       <c r="AQ35">
-        <v>56439535479</v>
+        <v>666333579</v>
       </c>
       <c r="AR35">
-        <v>56439535479</v>
+        <v>666333579</v>
       </c>
       <c r="AS35">
         <v>0</v>
@@ -5946,19 +5940,19 @@
         <v>0</v>
       </c>
       <c r="AV35">
-        <v>56439535479</v>
+        <v>666333579</v>
       </c>
       <c r="AW35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AX35">
-        <v>0.9619440335751347</v>
+        <v>0.01508300174160181</v>
       </c>
       <c r="AY35">
-        <v>58672369191</v>
+        <v>44177783071</v>
       </c>
       <c r="AZ35">
-        <v>0.9619440335751347</v>
+        <v>0.01508300174160181</v>
       </c>
     </row>
     <row r="36" spans="1:52">
@@ -5969,16 +5963,16 @@
         <v>53</v>
       </c>
       <c r="C36">
-        <v>20140101</v>
+        <v>20070101</v>
       </c>
       <c r="D36">
-        <v>2014</v>
+        <v>2007</v>
       </c>
       <c r="E36">
         <v>52</v>
       </c>
       <c r="F36" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G36">
         <v>24</v>
@@ -6014,7 +6008,7 @@
         <v>74</v>
       </c>
       <c r="R36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S36" t="s">
         <v>79</v>
@@ -6023,10 +6017,10 @@
         <v>1</v>
       </c>
       <c r="U36" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="V36" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="W36">
         <v>6</v>
@@ -6050,10 +6044,13 @@
         <v>114</v>
       </c>
       <c r="AD36">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="AE36" t="s">
-        <v>118</v>
+        <v>115</v>
+      </c>
+      <c r="AF36">
+        <v>7000343</v>
       </c>
       <c r="AG36" t="b">
         <v>0</v>
@@ -6067,6 +6064,9 @@
       <c r="AK36" t="b">
         <v>0</v>
       </c>
+      <c r="AL36">
+        <v>7000343</v>
+      </c>
       <c r="AM36" t="b">
         <v>0</v>
       </c>
@@ -6074,10 +6074,10 @@
         <v>0</v>
       </c>
       <c r="AQ36">
-        <v>1274009584</v>
+        <v>42575360</v>
       </c>
       <c r="AR36">
-        <v>1274009584</v>
+        <v>42575360</v>
       </c>
       <c r="AS36">
         <v>0</v>
@@ -6089,19 +6089,19 @@
         <v>0</v>
       </c>
       <c r="AV36">
-        <v>1274009584</v>
+        <v>42575360</v>
       </c>
       <c r="AW36">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AX36">
-        <v>0.02171396181143859</v>
+        <v>0.0009637278523364407</v>
       </c>
       <c r="AY36">
-        <v>58672369191</v>
+        <v>44177783071</v>
       </c>
       <c r="AZ36">
-        <v>0.02171396181143859</v>
+        <v>0.0009637278523364407</v>
       </c>
     </row>
     <row r="37" spans="1:52">
@@ -6166,10 +6166,10 @@
         <v>1</v>
       </c>
       <c r="U37" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="V37" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="W37">
         <v>6</v>
@@ -6470,10 +6470,10 @@
         <v>1</v>
       </c>
       <c r="U39" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="V39" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="W39">
         <v>6</v>
@@ -6622,10 +6622,10 @@
         <v>1</v>
       </c>
       <c r="U40" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="V40" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="W40">
         <v>6</v>
@@ -6926,10 +6926,10 @@
         <v>1</v>
       </c>
       <c r="U42" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="V42" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="W42">
         <v>6</v>
@@ -7075,10 +7075,10 @@
         <v>1</v>
       </c>
       <c r="U43" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="V43" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="W43">
         <v>6</v>
@@ -7373,10 +7373,10 @@
         <v>1</v>
       </c>
       <c r="U45" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="V45" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="W45">
         <v>6</v>
@@ -7677,10 +7677,10 @@
         <v>1</v>
       </c>
       <c r="U47" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="V47" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="W47">
         <v>6</v>
@@ -8273,10 +8273,10 @@
         <v>1</v>
       </c>
       <c r="U51" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="V51" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="W51">
         <v>6</v>
@@ -8732,10 +8732,10 @@
         <v>1</v>
       </c>
       <c r="U54" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="V54" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="W54">
         <v>6</v>
@@ -9039,10 +9039,10 @@
         <v>1</v>
       </c>
       <c r="U56" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="V56" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="W56">
         <v>6</v>
@@ -9501,10 +9501,10 @@
         <v>1</v>
       </c>
       <c r="U59" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="V59" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="W59">
         <v>6</v>
@@ -9656,10 +9656,10 @@
         <v>1</v>
       </c>
       <c r="U60" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="V60" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="W60">
         <v>6</v>
@@ -10121,10 +10121,10 @@
         <v>1</v>
       </c>
       <c r="U63" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="V63" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="W63">
         <v>6</v>
@@ -10276,10 +10276,10 @@
         <v>1</v>
       </c>
       <c r="U64" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="V64" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="W64">
         <v>6</v>
@@ -10741,10 +10741,10 @@
         <v>1</v>
       </c>
       <c r="U67" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="V67" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="W67">
         <v>6</v>
@@ -11206,10 +11206,10 @@
         <v>1</v>
       </c>
       <c r="U70" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="V70" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="W70">
         <v>6</v>
@@ -11516,10 +11516,10 @@
         <v>1</v>
       </c>
       <c r="U72" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="V72" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="W72">
         <v>6</v>
@@ -11549,25 +11549,25 @@
         <v>115</v>
       </c>
       <c r="AF72">
-        <v>62962811157</v>
+        <v>640411440</v>
       </c>
       <c r="AG72" t="b">
         <v>0</v>
       </c>
       <c r="AH72">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="AI72" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AJ72">
-        <v>395992523</v>
+        <v>640411.4399999999</v>
       </c>
       <c r="AK72" t="b">
         <v>0</v>
       </c>
       <c r="AL72">
-        <v>62962811157</v>
+        <v>640411440</v>
       </c>
       <c r="AM72" t="b">
         <v>0</v>
@@ -11579,10 +11579,10 @@
         <v>0</v>
       </c>
       <c r="AQ72">
-        <v>40311108896.754</v>
+        <v>480172846.807</v>
       </c>
       <c r="AR72">
-        <v>40311108896.754</v>
+        <v>480172846.807</v>
       </c>
       <c r="AS72">
         <v>0</v>
@@ -11594,19 +11594,19 @@
         <v>1</v>
       </c>
       <c r="AV72">
-        <v>40311108896.754</v>
+        <v>480172846.807</v>
       </c>
       <c r="AW72">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AX72">
-        <v>0.7861754628938258</v>
+        <v>0.009364666972431934</v>
       </c>
       <c r="AY72">
         <v>51274951711.636</v>
       </c>
       <c r="AZ72">
-        <v>0.7861754628938258</v>
+        <v>0.009364666972431934</v>
       </c>
     </row>
     <row r="73" spans="1:52">
@@ -11671,10 +11671,10 @@
         <v>1</v>
       </c>
       <c r="U73" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="V73" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="W73">
         <v>6</v>
@@ -11704,7 +11704,7 @@
         <v>115</v>
       </c>
       <c r="AF73">
-        <v>640411440</v>
+        <v>3570583100</v>
       </c>
       <c r="AG73" t="b">
         <v>0</v>
@@ -11716,13 +11716,13 @@
         <v>121</v>
       </c>
       <c r="AJ73">
-        <v>640411.4399999999</v>
+        <v>3570583.1</v>
       </c>
       <c r="AK73" t="b">
         <v>0</v>
       </c>
       <c r="AL73">
-        <v>640411440</v>
+        <v>3570583100</v>
       </c>
       <c r="AM73" t="b">
         <v>0</v>
@@ -11734,10 +11734,10 @@
         <v>0</v>
       </c>
       <c r="AQ73">
-        <v>480172846.807</v>
+        <v>6080727779.155</v>
       </c>
       <c r="AR73">
-        <v>480172846.807</v>
+        <v>6080727779.155</v>
       </c>
       <c r="AS73">
         <v>0</v>
@@ -11749,19 +11749,19 @@
         <v>1</v>
       </c>
       <c r="AV73">
-        <v>480172846.807</v>
+        <v>6080727779.155</v>
       </c>
       <c r="AW73">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AX73">
-        <v>0.009364666972431934</v>
+        <v>0.1185906095699955</v>
       </c>
       <c r="AY73">
         <v>51274951711.636</v>
       </c>
       <c r="AZ73">
-        <v>0.009364666972431934</v>
+        <v>0.1185906095699955</v>
       </c>
     </row>
     <row r="74" spans="1:52">
@@ -11826,10 +11826,10 @@
         <v>1</v>
       </c>
       <c r="U74" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="V74" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="W74">
         <v>6</v>
@@ -11853,31 +11853,31 @@
         <v>114</v>
       </c>
       <c r="AD74">
+        <v>-1</v>
+      </c>
+      <c r="AE74" t="s">
+        <v>118</v>
+      </c>
+      <c r="AF74">
+        <v>0</v>
+      </c>
+      <c r="AG74" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH74">
         <v>8</v>
       </c>
-      <c r="AE74" t="s">
+      <c r="AI74" t="s">
         <v>115</v>
       </c>
-      <c r="AF74">
-        <v>3570583100</v>
-      </c>
-      <c r="AG74" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH74">
-        <v>21</v>
-      </c>
-      <c r="AI74" t="s">
-        <v>121</v>
-      </c>
       <c r="AJ74">
-        <v>3570583.1</v>
+        <v>243845000</v>
       </c>
       <c r="AK74" t="b">
         <v>0</v>
       </c>
       <c r="AL74">
-        <v>3570583100</v>
+        <v>243845000</v>
       </c>
       <c r="AM74" t="b">
         <v>0</v>
@@ -11889,10 +11889,10 @@
         <v>0</v>
       </c>
       <c r="AQ74">
-        <v>6080727779.155</v>
+        <v>440944058.478</v>
       </c>
       <c r="AR74">
-        <v>6080727779.155</v>
+        <v>440944058.478</v>
       </c>
       <c r="AS74">
         <v>0</v>
@@ -11904,19 +11904,19 @@
         <v>1</v>
       </c>
       <c r="AV74">
-        <v>6080727779.155</v>
+        <v>440944058.478</v>
       </c>
       <c r="AW74">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AX74">
-        <v>0.1185906095699955</v>
+        <v>0.008599599682859088</v>
       </c>
       <c r="AY74">
         <v>51274951711.636</v>
       </c>
       <c r="AZ74">
-        <v>0.1185906095699955</v>
+        <v>0.008599599682859088</v>
       </c>
     </row>
     <row r="75" spans="1:52">
@@ -11981,10 +11981,10 @@
         <v>1</v>
       </c>
       <c r="U75" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="V75" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="W75">
         <v>6</v>
@@ -12136,10 +12136,10 @@
         <v>1</v>
       </c>
       <c r="U76" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="V76" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="W76">
         <v>6</v>
@@ -12163,31 +12163,31 @@
         <v>114</v>
       </c>
       <c r="AD76">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="AE76" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="AF76">
-        <v>0</v>
+        <v>62962811157</v>
       </c>
       <c r="AG76" t="b">
         <v>0</v>
       </c>
       <c r="AH76">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="AI76" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="AJ76">
-        <v>243845000</v>
+        <v>395992523</v>
       </c>
       <c r="AK76" t="b">
         <v>0</v>
       </c>
       <c r="AL76">
-        <v>243845000</v>
+        <v>62962811157</v>
       </c>
       <c r="AM76" t="b">
         <v>0</v>
@@ -12199,10 +12199,10 @@
         <v>0</v>
       </c>
       <c r="AQ76">
-        <v>440944058.478</v>
+        <v>40311108896.754</v>
       </c>
       <c r="AR76">
-        <v>440944058.478</v>
+        <v>40311108896.754</v>
       </c>
       <c r="AS76">
         <v>0</v>
@@ -12214,19 +12214,19 @@
         <v>1</v>
       </c>
       <c r="AV76">
-        <v>440944058.478</v>
+        <v>40311108896.754</v>
       </c>
       <c r="AW76">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AX76">
-        <v>0.008599599682859088</v>
+        <v>0.7861754628938258</v>
       </c>
       <c r="AY76">
         <v>51274951711.636</v>
       </c>
       <c r="AZ76">
-        <v>0.008599599682859088</v>
+        <v>0.7861754628938258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>